<commit_message>
hours calculation - not yet tested
</commit_message>
<xml_diff>
--- a/Documentation/Open Issues.xlsx
+++ b/Documentation/Open Issues.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Open Issues</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>High</t>
+  </si>
+  <si>
+    <t>Shortlist product when program is selected on "Test" page</t>
   </si>
 </sst>
 </file>
@@ -145,7 +148,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -158,12 +161,12 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="7" tint="0.39994506668294322"/>
+        <color theme="7" tint="-0.24994659260841701"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <color theme="4" tint="0.39994506668294322"/>
+        <color theme="4" tint="-0.24994659260841701"/>
       </font>
     </dxf>
     <dxf>
@@ -183,161 +186,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -619,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -744,34 +592,40 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>8</v>
       </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Incomplete"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Moderate"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>